<commit_message>
Added code to handle alert
</commit_message>
<xml_diff>
--- a/TestData/Book1.xlsx
+++ b/TestData/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venga\PycharmProjects\SauceDemoAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venga\PycharmProjects\SauceDemoAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E445B5F-37C0-44D3-8123-8DE0C156C878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ACD836-B2A1-41DB-8698-A1DD69B904CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F957413-C491-47F2-A76F-BEFA126C558B}"/>
   </bookViews>
@@ -34,18 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Sauce Labs Backpack</t>
-  </si>
-  <si>
-    <t>Sauce Labs Bike Light</t>
-  </si>
-  <si>
-    <t>Sauce Labs Bolt T-Shirt</t>
   </si>
   <si>
     <t>Sauce Labs Onesie</t>
@@ -400,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0788DE84-3871-4E5D-B428-423DB5153E98}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,21 +412,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>